<commit_message>
Added ratings to meals 2
</commit_message>
<xml_diff>
--- a/meals.xlsx
+++ b/meals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="meals" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="155">
   <si>
     <t>MealID</t>
   </si>
@@ -474,6 +474,12 @@
   </si>
   <si>
     <t>Romano cheese</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>falafel mix</t>
   </si>
 </sst>
 </file>
@@ -834,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,10 +852,10 @@
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -868,8 +874,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -888,8 +897,11 @@
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -908,8 +920,11 @@
       <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -928,8 +943,11 @@
       <c r="F4" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -948,8 +966,11 @@
       <c r="F5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -968,8 +989,11 @@
       <c r="F6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -988,8 +1012,11 @@
       <c r="F7" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1008,8 +1035,11 @@
       <c r="F8" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1028,8 +1058,11 @@
       <c r="F9" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1048,8 +1081,11 @@
       <c r="F10" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1068,8 +1104,11 @@
       <c r="F11" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1088,8 +1127,11 @@
       <c r="F12" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1108,8 +1150,11 @@
       <c r="F13" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1128,8 +1173,11 @@
       <c r="F14" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1148,8 +1196,11 @@
       <c r="F15" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1168,8 +1219,11 @@
       <c r="F16" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1188,8 +1242,11 @@
       <c r="F17" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1208,8 +1265,11 @@
       <c r="F18" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1228,8 +1288,11 @@
       <c r="F19" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1248,8 +1311,11 @@
       <c r="F20" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1268,8 +1334,11 @@
       <c r="F21" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1288,8 +1357,11 @@
       <c r="F22" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1308,8 +1380,11 @@
       <c r="F23" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1328,8 +1403,11 @@
       <c r="F24" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1346,8 +1424,11 @@
       <c r="F25" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1366,8 +1447,11 @@
       <c r="F26" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1386,8 +1470,11 @@
       <c r="F27" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1406,8 +1493,11 @@
       <c r="F28" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1426,8 +1516,11 @@
       <c r="F29" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1442,10 +1535,13 @@
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1464,8 +1560,11 @@
       <c r="F31" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1484,8 +1583,11 @@
       <c r="F32" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1504,8 +1606,11 @@
       <c r="F33" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1524,8 +1629,11 @@
       <c r="F34" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1544,8 +1652,11 @@
       <c r="F35" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1564,6 +1675,17 @@
       <c r="F36" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1575,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,73 +1728,95 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
@@ -1687,52 +1831,52 @@
         <v>97</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>141</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>91</v>
+        <v>146</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>95</v>
+        <v>25</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>143</v>
+        <v>80</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>141</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>108</v>
@@ -1742,91 +1886,91 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>141</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>102</v>
+        <v>25</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>141</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>145</v>
+        <v>101</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>110</v>
+        <v>28</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>146</v>
+        <v>80</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>108</v>
@@ -1836,30 +1980,32 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="D18" s="2" t="s">
-        <v>147</v>
+        <v>104</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="2">
-        <v>2</v>
+        <v>28</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1872,761 +2018,779 @@
         <v>28</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="2">
-        <v>1</v>
+        <v>49</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>102</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C23" s="2">
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>102</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>102</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>102</v>
+        <v>35</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>139</v>
+        <v>77</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>102</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="2">
-        <v>2</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>122</v>
+        <v>26</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
       <c r="D31" s="2" t="s">
-        <v>140</v>
+        <v>72</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>97</v>
+        <v>38</v>
+      </c>
+      <c r="C33" s="2">
+        <v>40</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>124</v>
+        <v>13</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="2">
-        <v>3</v>
+        <v>50</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="C37" s="2">
+        <v>2</v>
+      </c>
       <c r="D37" s="2" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
       <c r="D38" s="2" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C40" s="2">
         <v>1</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>73</v>
+        <v>51</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" s="2">
-        <v>40</v>
+        <v>51</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="C43" s="2">
+        <v>3</v>
+      </c>
       <c r="D43" s="2" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="D44" s="2" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>75</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" s="2">
-        <v>2</v>
+        <v>51</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C47" s="2">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C48" s="2">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C49" s="2">
         <v>1</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C50" s="2">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>81</v>
+        <v>59</v>
+      </c>
+      <c r="C51" s="2">
+        <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C52" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C54" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="C54" s="2">
+        <v>2</v>
+      </c>
       <c r="D54" s="2" t="s">
-        <v>26</v>
+        <v>108</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>83</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>91</v>
+        <v>14</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="C58" s="2">
+        <v>1</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="C59" s="2">
+        <v>1</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="C60" s="2">
+        <v>3</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
+      <c r="D61" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C62" s="2">
-        <v>1</v>
+        <v>53</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C64" s="2">
-        <v>1</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C65" s="2">
-        <v>1</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C67" s="2">
-        <v>2</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
-        <v>108</v>
+        <v>26</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C68" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="C68" s="2">
+        <v>1</v>
+      </c>
       <c r="D68" s="2" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>99</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>14</v>
@@ -2636,320 +2800,322 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C71" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C72" s="2">
         <v>1</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C73" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C74" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="D74" s="2" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>110</v>
+        <v>61</v>
+      </c>
+      <c r="C75" s="2">
+        <v>2</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C77" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="D77" s="2" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C80" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="D80" s="2" t="s">
-        <v>26</v>
+        <v>133</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C81" s="2">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>80</v>
+        <v>135</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C82" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="C82" s="2">
+        <v>2</v>
+      </c>
       <c r="D82" s="2" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>119</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C83" s="2"/>
       <c r="D83" s="2" t="s">
-        <v>14</v>
+        <v>124</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C84" s="2">
-        <v>3</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C84" s="2"/>
       <c r="D84" s="2" t="s">
-        <v>108</v>
+        <v>46</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C85" s="2">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>120</v>
+        <v>148</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C86" s="2">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>102</v>
+        <v>63</v>
+      </c>
+      <c r="C87" s="2">
+        <v>2</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C88" s="2">
-        <v>2</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C88" s="2"/>
       <c r="D88" s="2" t="s">
-        <v>122</v>
+        <v>151</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>87</v>
+        <v>66</v>
+      </c>
+      <c r="C90" s="2">
+        <v>2</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2" t="s">
@@ -2960,180 +3126,164 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>130</v>
+        <v>66</v>
+      </c>
+      <c r="C92" s="2">
+        <v>1</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>132</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C93" s="2"/>
       <c r="D93" s="2" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
+        <v>31</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C95" s="2">
-        <v>2</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C96" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="C96" s="2">
+        <v>3</v>
+      </c>
       <c r="D96" s="2" t="s">
-        <v>124</v>
+        <v>77</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E97" s="2"/>
-      <c r="F97" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="D98" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="D99" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C100" s="2">
-        <v>2</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="C100" t="s">
+        <v>95</v>
+      </c>
+      <c r="D100" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C101" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="D101" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>152</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
@@ -3142,10 +3292,10 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
@@ -3154,10 +3304,10 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
@@ -3166,116 +3316,94 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C106" s="2">
-        <v>2</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>108</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="C107" s="2"/>
-      <c r="D107" s="2" t="s">
-        <v>126</v>
-      </c>
+      <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C108" s="2">
-        <v>1</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>136</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="C109" s="2"/>
-      <c r="D109" s="2" t="s">
-        <v>124</v>
-      </c>
+      <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>138</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C111" s="2"/>
-      <c r="D111" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C112" s="2">
-        <v>3</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>77</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
@@ -3284,10 +3412,10 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
@@ -3296,10 +3424,10 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
@@ -3308,53 +3436,51 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C116">
-        <v>1</v>
-      </c>
-      <c r="D116" t="s">
-        <v>72</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D117" t="s">
-        <v>93</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D118" t="s">
-        <v>94</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C118" s="2"/>
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C119" t="s">
-        <v>95</v>
-      </c>
-      <c r="D119" t="s">
-        <v>96</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>